<commit_message>
Updated ProjectDB, Project class
</commit_message>
<xml_diff>
--- a/App/data/rollover_project.xlsx
+++ b/App/data/rollover_project.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugen\Desktop\Coding\Coding Projects\Github Repo\OOP-FYP-Management-Project\App\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51AFD05-0D72-4BEF-B92F-ED668D1F1CFD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE012DE-27B5-4225-A428-671A4FFA18A0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>Title</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>StudentID</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -466,7 +469,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,7 +502,9 @@
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="D2" s="4" t="s">
         <v>19</v>
       </c>
@@ -515,6 +520,9 @@
       <c r="D3" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -527,6 +535,9 @@
       <c r="D4" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -539,6 +550,9 @@
       <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -551,6 +565,9 @@
       <c r="D6" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -563,6 +580,9 @@
       <c r="D7" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -575,6 +595,9 @@
       <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -587,6 +610,9 @@
       <c r="D9" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -599,6 +625,9 @@
       <c r="D10" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -611,6 +640,9 @@
       <c r="D11" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -623,6 +655,9 @@
       <c r="D12" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -635,6 +670,9 @@
       <c r="D13" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -647,6 +685,9 @@
       <c r="D14" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -659,6 +700,9 @@
       <c r="D15" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -671,8 +715,11 @@
       <c r="D16" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -682,6 +729,9 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
         <v>29</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing Bugs in RequestDB
</commit_message>
<xml_diff>
--- a/App/data/rollover_project.xlsx
+++ b/App/data/rollover_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugen\Desktop\Coding\Coding Projects\Github Repo\OOP-FYP-Management-Project\App\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A555D19B-E135-46AF-8DD7-17E26B325309}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F373C6A-BCD3-412F-BEEB-F5241CC98821}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
   <si>
     <t>Title</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>AVAILABLE</t>
   </si>
 </sst>
 </file>
@@ -472,7 +475,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E2" sqref="E2:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,7 +518,9 @@
       <c r="D2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -528,7 +533,9 @@
       <c r="D3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="F3" t="s">
         <v>32</v>
       </c>
@@ -544,7 +551,9 @@
       <c r="D4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="F4" t="s">
         <v>32</v>
       </c>
@@ -560,7 +569,9 @@
       <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="F5" t="s">
         <v>32</v>
       </c>
@@ -576,7 +587,9 @@
       <c r="D6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="F6" t="s">
         <v>32</v>
       </c>
@@ -592,7 +605,9 @@
       <c r="D7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="F7" t="s">
         <v>32</v>
       </c>
@@ -608,7 +623,9 @@
       <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="F8" t="s">
         <v>32</v>
       </c>
@@ -624,7 +641,9 @@
       <c r="D9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="F9" t="s">
         <v>32</v>
       </c>
@@ -640,7 +659,9 @@
       <c r="D10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="F10" t="s">
         <v>32</v>
       </c>
@@ -656,7 +677,9 @@
       <c r="D11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="F11" t="s">
         <v>32</v>
       </c>
@@ -672,7 +695,9 @@
       <c r="D12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="F12" t="s">
         <v>32</v>
       </c>
@@ -688,7 +713,9 @@
       <c r="D13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="F13" t="s">
         <v>32</v>
       </c>
@@ -704,7 +731,9 @@
       <c r="D14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="F14" t="s">
         <v>32</v>
       </c>
@@ -720,7 +749,9 @@
       <c r="D15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="F15" t="s">
         <v>32</v>
       </c>
@@ -736,7 +767,9 @@
       <c r="D16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="F16" t="s">
         <v>32</v>
       </c>
@@ -752,7 +785,9 @@
       <c r="D17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="F17" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Updated EnactRequest Class, Supervisor ManageR
</commit_message>
<xml_diff>
--- a/App/data/rollover_project.xlsx
+++ b/App/data/rollover_project.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clare/Documents/GitHub/OOP-FYP-Management-Project/App/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugen\Desktop\Coding\Coding Projects\Github Repo\OOP-FYP-Management-Project\App\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE61274-9566-214E-BE98-F892E20FBF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F373C6A-BCD3-412F-BEEB-F5241CC98821}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="39">
   <si>
     <t>Title</t>
   </si>
@@ -132,14 +132,24 @@
     <t>AVAILABLE</t>
   </si>
   <si>
+    <t>testing1</t>
+  </si>
+  <si>
     <t>newtitle1</t>
+  </si>
+  <si>
+    <t>testing2</t>
+  </si>
+  <si>
+    <t>newtitle2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +159,12 @@
     </font>
     <font>
       <b/>
+      <sz val="9"/>
+      <color indexed="64"/>
+      <name val="Microsoft Sans Serif"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color indexed="64"/>
       <name val="Microsoft Sans Serif"/>
@@ -183,9 +199,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -467,21 +485,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E2" sqref="E2:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="74.5" customWidth="1"/>
-    <col min="3" max="4" width="32.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="74.44140625"/>
+    <col min="3" max="4" customWidth="true" width="32.6640625"/>
+    <col min="5" max="5" customWidth="true" width="10.109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -496,296 +514,367 @@
       <c r="E1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="E2" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="E3" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C4" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="E4" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C5" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="E5" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C6" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="E6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="E6" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C7" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="E7" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C8" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="E8" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="n" s="0">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C9" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="E9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="E9" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C10" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="E10" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C11" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="E11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="E11" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="n" s="0">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C12" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="E12" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B13" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C13" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="E13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="E13" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="n" s="0">
+        <v>13.0</v>
+      </c>
+      <c r="B14" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="C14" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="E14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="E14" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F14" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="n" s="0">
+        <v>14.0</v>
+      </c>
+      <c r="B15" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C15" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="E15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="E15" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F15" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="n" s="0">
+        <v>15.0</v>
+      </c>
+      <c r="B16" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C16" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="E16" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="E16" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F16" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="n" s="0">
+        <v>16.0</v>
+      </c>
+      <c r="B17" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C17" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="E17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E17" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F17" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n" s="0">
+        <v>17.0</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="E18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="E18" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F18" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n" s="0">
+        <v>18.0</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E19" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F19" t="s" s="0">
         <v>32</v>
       </c>
     </row>

</xml_diff>